<commit_message>
feat: add invoice status filter and overview export; fix relational list phone/total
- Add status (Oui/Non) filter in QueryBuilder and Search UI\n- Show canceled status in invoice overview; export general_status (ODT/XLSX)\n- Include supplier phone in relational exports; add total/total_supplier for XLSX
</commit_message>
<xml_diff>
--- a/server/templates/excel/invoice/invoice-overview.xlsx
+++ b/server/templates/excel/invoice/invoice-overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\WebstormProjects\invoice-app\server\templates\excel\invoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F754079-1E95-4CD4-B79D-88B5A3B0FF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF87ACD-8FE5-4688-BCDE-47FA4E855DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Facture</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>{d.invoice.fiscal_year}</t>
+  </si>
+  <si>
+    <t>Etat Facture :</t>
+  </si>
+  <si>
+    <t>{d.invoice.general_status}</t>
   </si>
 </sst>
 </file>
@@ -379,7 +385,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,6 +440,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -485,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -801,6 +813,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1180,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="110" zoomScaleNormal="90" zoomScaleSheetLayoutView="117" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="110" zoomScaleNormal="90" zoomScaleSheetLayoutView="117" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1403,8 +1418,12 @@
       <c r="C12" s="70"/>
       <c r="D12" s="70"/>
       <c r="E12" s="97"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
+      <c r="F12" s="82" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="82" t="s">
+        <v>50</v>
+      </c>
       <c r="H12" s="67"/>
       <c r="I12" s="51"/>
       <c r="J12" s="41"/>
@@ -1423,8 +1442,8 @@
       <c r="C13" s="70"/>
       <c r="D13" s="70"/>
       <c r="E13" s="97"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="100"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
       <c r="H13" s="100"/>
       <c r="I13" s="51"/>
       <c r="J13" s="39"/>

</xml_diff>